<commit_message>
Updated multiple management files to have consistent and english values.
</commit_message>
<xml_diff>
--- a/data/management/Management_information_GGE_2015.xlsx
+++ b/data/management/Management_information_GGE_2015.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tillrose/Library/Mobile Documents/com~apple~CloudDocs/iCloud Daten/Arbeit/R-Projects/Git_Repositories/BRIWECS_Data_Publication_2/data/management/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3B097E-DCFF-294A-8E27-66EFE552EBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32240" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
@@ -265,9 +271,6 @@
     <t>Ernte vom 28.07-03,08</t>
   </si>
   <si>
-    <t>KAS</t>
-  </si>
-  <si>
     <t>70gr/ha+ 1l/ha+1,2l/ha+20gr/ha</t>
   </si>
   <si>
@@ -302,13 +305,16 @@
   </si>
   <si>
     <t>27.10/28.10.2014</t>
+  </si>
+  <si>
+    <t>CAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,10 +518,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="20% - Akzent3" xfId="3" builtinId="38"/>
-    <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
-    <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -531,9 +537,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -571,7 +577,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -605,6 +611,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -639,9 +646,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -814,33 +822,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
-    <col min="11" max="11" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="50.5" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="27.5" customWidth="1"/>
+    <col min="9" max="9" width="28.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" customWidth="1"/>
+    <col min="11" max="11" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="34.5" customHeight="1">
+    <row r="1" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -848,7 +856,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -856,25 +864,25 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -882,7 +890,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -890,7 +898,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -898,19 +906,19 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="12" spans="1:2" ht="45.75" customHeight="1">
+    <row r="12" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -918,7 +926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -926,7 +934,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -934,7 +942,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -942,21 +950,21 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="53.25" customHeight="1">
+    <row r="18" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -965,7 +973,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -974,7 +982,7 @@
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -983,18 +991,18 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1003,16 +1011,16 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -1021,7 +1029,7 @@
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1030,28 +1038,28 @@
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1070,7 @@
         <v>41960</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
@@ -1073,7 +1081,7 @@
         <v>41960</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
@@ -1084,7 +1092,7 @@
         <v>41960</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
@@ -1095,14 +1103,14 @@
         <v>41960</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -1113,7 +1121,7 @@
         <v>42080</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
@@ -1124,7 +1132,7 @@
         <v>42080</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
@@ -1135,7 +1143,7 @@
         <v>42080</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
@@ -1146,14 +1154,14 @@
         <v>42080</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="46.5" customHeight="1">
+    <row r="42" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>68</v>
       </c>
@@ -1168,7 +1176,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" ht="24" customHeight="1">
+    <row r="43" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>54</v>
       </c>
@@ -1203,7 +1211,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1217,7 +1225,7 @@
         <v>40</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>13</v>
@@ -1226,17 +1234,17 @@
         <v>42102</v>
       </c>
       <c r="H44" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K44" s="8"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1250,7 +1258,7 @@
         <v>23</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>14</v>
@@ -1263,7 +1271,7 @@
       </c>
       <c r="K45" s="8"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -1284,7 +1292,7 @@
       </c>
       <c r="K46" s="8"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1305,7 +1313,7 @@
       </c>
       <c r="K47" s="8"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -1324,7 +1332,7 @@
       </c>
       <c r="K48" s="8"/>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1343,7 +1351,7 @@
       </c>
       <c r="K49" s="8"/>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -1360,7 +1368,7 @@
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1377,7 +1385,7 @@
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1394,7 +1402,7 @@
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
     </row>
-    <row r="54" spans="1:11" ht="36" customHeight="1">
+    <row r="54" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
         <v>54</v>
       </c>
@@ -1429,7 +1437,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -1443,7 +1451,7 @@
         <v>50</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>13</v>
@@ -1452,17 +1460,17 @@
         <v>42102</v>
       </c>
       <c r="H55" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I55" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="I55" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="J55" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K55" s="8"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1476,7 +1484,7 @@
         <v>63</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>14</v>
@@ -1489,7 +1497,7 @@
       </c>
       <c r="K56" s="8"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -1503,7 +1511,7 @@
         <v>60</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>15</v>
@@ -1516,7 +1524,7 @@
       </c>
       <c r="K57" s="8"/>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -1537,7 +1545,7 @@
       </c>
       <c r="K58" s="8"/>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -1556,7 +1564,7 @@
       </c>
       <c r="K59" s="8"/>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -1575,7 +1583,7 @@
       </c>
       <c r="K60" s="8"/>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -1592,7 +1600,7 @@
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -1607,15 +1615,15 @@
         <v>42104</v>
       </c>
       <c r="H62" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I62" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="I62" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -1632,7 +1640,7 @@
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
     </row>
-    <row r="65" spans="1:11" ht="37.5" customHeight="1">
+    <row r="65" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>54</v>
       </c>
@@ -1667,7 +1675,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -1681,7 +1689,7 @@
         <v>50</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F66" s="7" t="s">
         <v>13</v>
@@ -1690,17 +1698,17 @@
         <v>42102</v>
       </c>
       <c r="H66" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I66" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="I66" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="J66" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K66" s="8"/>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -1714,7 +1722,7 @@
         <v>63</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>14</v>
@@ -1727,7 +1735,7 @@
       </c>
       <c r="K67" s="8"/>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -1741,7 +1749,7 @@
         <v>60</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F68" s="7" t="s">
         <v>15</v>
@@ -1754,7 +1762,7 @@
       </c>
       <c r="K68" s="8"/>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -1775,7 +1783,7 @@
       </c>
       <c r="K69" s="8"/>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1790,17 +1798,17 @@
         <v>42118</v>
       </c>
       <c r="H70" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I70" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="I70" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="J70" s="8" t="s">
         <v>62</v>
       </c>
       <c r="K70" s="8"/>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1815,17 +1823,17 @@
         <v>42147</v>
       </c>
       <c r="H71" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I71" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="I71" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="J71" s="8" t="s">
         <v>63</v>
       </c>
       <c r="K71" s="8"/>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -1842,7 +1850,7 @@
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>69</v>
       </c>
@@ -1857,15 +1865,15 @@
         <v>42104</v>
       </c>
       <c r="H73" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I73" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="I73" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>69</v>
       </c>
@@ -1882,7 +1890,7 @@
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>54</v>
       </c>
@@ -1917,7 +1925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -1931,7 +1939,7 @@
         <v>50</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>13</v>
@@ -1940,17 +1948,17 @@
         <v>42102</v>
       </c>
       <c r="H77" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I77" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="I77" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="J77" s="8" t="s">
         <v>58</v>
       </c>
       <c r="K77" s="8"/>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -1964,7 +1972,7 @@
         <v>63</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>14</v>
@@ -1977,7 +1985,7 @@
       </c>
       <c r="K78" s="8"/>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>73</v>
       </c>
@@ -1991,7 +1999,7 @@
         <v>60</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F79" s="7" t="s">
         <v>15</v>
@@ -2004,7 +2012,7 @@
       </c>
       <c r="K79" s="8"/>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>73</v>
       </c>
@@ -2025,7 +2033,7 @@
       </c>
       <c r="K80" s="8"/>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>73</v>
       </c>
@@ -2040,17 +2048,17 @@
         <v>42118</v>
       </c>
       <c r="H81" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I81" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="I81" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="J81" s="8" t="s">
         <v>62</v>
       </c>
       <c r="K81" s="8"/>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>73</v>
       </c>
@@ -2065,17 +2073,17 @@
         <v>42147</v>
       </c>
       <c r="H82" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I82" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="I82" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="J82" s="8" t="s">
         <v>63</v>
       </c>
       <c r="K82" s="8"/>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>73</v>
       </c>
@@ -2092,7 +2100,7 @@
       <c r="J83" s="8"/>
       <c r="K83" s="8"/>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>73</v>
       </c>
@@ -2107,15 +2115,15 @@
         <v>42104</v>
       </c>
       <c r="H84" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I84" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="I84" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>73</v>
       </c>
@@ -2132,24 +2140,24 @@
       <c r="J85" s="8"/>
       <c r="K85" s="8"/>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>